<commit_message>
docs update and met_mast_reader renamed
</commit_message>
<xml_diff>
--- a/Examples/SCADA_reader/SVI_Definition.xlsx
+++ b/Examples/SCADA_reader/SVI_Definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PhD\Codes\GitLab\tum_plc_linker\Examples\SCADA_reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PhD\Codes\Github\PAL\Examples\SCADA_reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E559D9C-198B-4799-99BE-C479DAD895DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84A66E4-EF74-4650-962E-83F2F6C4D418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ITFC" sheetId="1" r:id="rId1"/>
@@ -716,7 +716,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1108,12 +1108,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -1121,7 +1121,7 @@
     <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" s="2" customFormat="1">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>3</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>3</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>3</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>3</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>3</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" s="2" customFormat="1">
       <c r="A50" s="2">
         <v>4</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" s="2" customFormat="1">
       <c r="A51" s="2">
         <v>5</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" s="2" customFormat="1">
       <c r="A52" s="2">
         <v>6</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" s="2" customFormat="1">
       <c r="A53" s="2">
         <v>7</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>7</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>7</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>7</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>7</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>7</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>7</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" s="2" customFormat="1">
       <c r="A62" s="2">
         <v>8</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>8</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>8</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>8</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>8</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>8</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68">
         <v>8</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69">
         <v>8</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8">
       <c r="A70">
         <v>8</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71">
         <v>8</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72">
         <v>8</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73">
         <v>8</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8">
       <c r="A74">
         <v>8</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8">
       <c r="A75">
         <v>8</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8">
       <c r="A76">
         <v>8</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8">
       <c r="A77">
         <v>8</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8">
       <c r="A78">
         <v>8</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8">
       <c r="A79">
         <v>8</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8">
       <c r="A80">
         <v>8</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8">
       <c r="A81">
         <v>8</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" s="2" customFormat="1">
       <c r="A82" s="2">
         <v>9</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" s="2" customFormat="1">
       <c r="A83" s="2">
         <v>10</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8">
       <c r="A84">
         <v>10</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8">
       <c r="A85">
         <v>10</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8">
       <c r="A86">
         <v>10</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8">
       <c r="A87">
         <v>10</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8">
       <c r="A88">
         <v>10</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8">
       <c r="A89">
         <v>10</v>
       </c>
@@ -2976,12 +2976,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04924C5-A102-4AD2-85B4-C24CF21F5397}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -2994,7 +2994,7 @@
     <col min="15" max="15" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -4219,7 +4219,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>117</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>119</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>122</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -4830,7 +4830,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>126</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>127</v>
       </c>
@@ -4924,7 +4924,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>128</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>129</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>130</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>131</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>132</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>133</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>134</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>135</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>136</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>137</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>138</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>139</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15">
       <c r="A54" t="s">
         <v>140</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>142</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>143</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>144</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>145</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>146</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>147</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15">
       <c r="A63" t="s">
         <v>149</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>159</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>69</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -6569,7 +6569,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -6804,7 +6804,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>221</v>
       </c>
@@ -6898,7 +6898,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>222</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>223</v>
       </c>
@@ -6992,7 +6992,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" s="3" customFormat="1">
       <c r="A86" s="3" t="s">
         <v>150</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="3" customFormat="1">
       <c r="A87" s="3" t="s">
         <v>151</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="3" customFormat="1">
       <c r="A88" s="3" t="s">
         <v>152</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="3" customFormat="1">
       <c r="A89" s="3" t="s">
         <v>153</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="3" customFormat="1">
       <c r="A90" s="3" t="s">
         <v>154</v>
       </c>
@@ -7227,7 +7227,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="3" customFormat="1">
       <c r="A91" s="3" t="s">
         <v>155</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="3" customFormat="1">
       <c r="A92" s="3" t="s">
         <v>156</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>82</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
         <v>83</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15">
       <c r="A95" t="s">
         <v>84</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15">
       <c r="A96" t="s">
         <v>85</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>86</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>87</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="99" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" s="2" customFormat="1">
       <c r="A99" s="2" t="s">
         <v>189</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="100" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" s="2" customFormat="1">
       <c r="A100" s="2" t="s">
         <v>191</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="101" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" s="2" customFormat="1">
       <c r="A101" s="2" t="s">
         <v>192</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" s="2" customFormat="1">
       <c r="A102" s="2" t="s">
         <v>190</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" s="2" customFormat="1">
       <c r="A103" s="2" t="s">
         <v>193</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="104" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" s="2" customFormat="1">
       <c r="A104" s="2" t="s">
         <v>195</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="105" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" s="2" customFormat="1">
       <c r="A105" s="2" t="s">
         <v>196</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15">
       <c r="A106" s="2" t="s">
         <v>214</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15">
       <c r="A107" s="2" t="s">
         <v>224</v>
       </c>
@@ -7933,7 +7933,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
@@ -7946,7 +7946,7 @@
     <col min="12" max="12" width="22.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -8022,7 +8022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>177</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>177</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>177</v>
       </c>
@@ -8174,7 +8174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>177</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>177</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -8288,7 +8288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>177</v>
       </c>
@@ -8362,7 +8362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>198</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>198</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>198</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>198</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>198</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>198</v>
       </c>
@@ -8818,7 +8818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>198</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>198</v>
       </c>
@@ -8894,7 +8894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>198</v>
       </c>
@@ -8932,7 +8932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -9082,7 +9082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>215</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>215</v>
       </c>

</xml_diff>